<commit_message>
Release v2.0: Shared prompts, GDP per capita, provider auto-detection, and enhanced README
Major release with centralized prompt templates for all 8 LLM providers, GDP per capita field for countries, provider auto-detection in country-info CLI, database numeric precision fixes, architecture documentation with Mermaid diagrams, and comprehensive README linking to runbook.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/countries/countries.xlsx
+++ b/countries/countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sudipto\Projects-external\AIML_projects\llm-interactions-for-structured-outputs\countries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8D89B0-A631-41C3-9C2D-983A377FDE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD33CCA6-9E07-44CC-B3CC-904837257577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21636" yWindow="-2220" windowWidth="19200" windowHeight="11184" xr2:uid="{51401DFC-0B90-4182-B24E-913B83661CE5}"/>
+    <workbookView xWindow="38745" yWindow="855" windowWidth="20415" windowHeight="13530" xr2:uid="{51401DFC-0B90-4182-B24E-913B83661CE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,32 +903,32 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -937,58 +937,58 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -997,58 +997,58 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>